<commit_message>
last update before handing in
* updated overview with some comments on chapter 2
* added folder with all files sent for first presentation
</commit_message>
<xml_diff>
--- a/Overview implementations.xlsx
+++ b/Overview implementations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
   <si>
     <t>2</t>
   </si>
@@ -276,6 +276,21 @@
   </si>
   <si>
     <t>send advertisements at rate 1/3rd of lifetime in icmp header or faster</t>
+  </si>
+  <si>
+    <t>Set routing table to home network , then deregister the old CareOfAddress</t>
+  </si>
+  <si>
+    <t>check if R-bit (15) set to 1, if so, register with FA, else discard</t>
+  </si>
+  <si>
+    <t>only generate request packet if new sequence number &lt; old sequence number and new sequence number &lt; 255</t>
+  </si>
+  <si>
+    <t>start timer when receiving advertisement, restart timer when receiving another advertisement, send solicitation when timer runs out</t>
+  </si>
+  <si>
+    <t>when FA/HA receive solicitation, send advertisement</t>
   </si>
 </sst>
 </file>
@@ -670,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8">
         <v>2</v>
@@ -872,7 +887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3">
         <v>3</v>
@@ -882,8 +897,11 @@
       <c r="E18" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -894,7 +912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8">
@@ -905,7 +923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>4</v>
       </c>
@@ -913,15 +931,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>2</v>
       </c>
@@ -929,31 +950,40 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>3</v>
       </c>
       <c r="E25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -961,7 +991,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>1</v>
       </c>
@@ -969,7 +999,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>3</v>
       </c>
@@ -977,7 +1007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>4</v>
       </c>
@@ -985,7 +1015,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>6</v>
       </c>
@@ -993,7 +1023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>1</v>
       </c>

</xml_diff>